<commit_message>
benetech/ServiceNet#1608: LinkForCare Service Available 24/7
</commit_message>
<xml_diff>
--- a/src/test/resources/adapters/linkforcare/complete.xlsx
+++ b/src/test/resources/adapters/linkforcare/complete.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="814">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="818">
   <si>
     <t xml:space="preserve">ADA_PARATRANSIT__C</t>
   </si>
@@ -2189,6 +2189,12 @@
     <t xml:space="preserve">2019-04-03T19:19:19.000Z</t>
   </si>
   <si>
+    <t xml:space="preserve">status details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">status formula</t>
+  </si>
+  <si>
     <t xml:space="preserve">asda,sdas,das,das,d</t>
   </si>
   <si>
@@ -2213,6 +2219,9 @@
     <t xml:space="preserve">Sunday: CLOSED&lt;br&gt;Monday: 8:00 AM to 4:30 PM&lt;br&gt;Tuesday: 8:00 AM to 4:30 PM&lt;br&gt;Wednesday: 8:00 AM to 4:30 PM&lt;br&gt;Thursday: 8:00 AM to 4:30 PM&lt;br&gt;Friday: 8:00 AM to 4:30 PM&lt;br&gt;Saturday: CLOSED&lt;br&gt;</t>
   </si>
   <si>
+    <t xml:space="preserve">application process</t>
+  </si>
+  <si>
     <t xml:space="preserve">aaaas2232</t>
   </si>
   <si>
@@ -2253,6 +2262,9 @@
   </si>
   <si>
     <t xml:space="preserve">asdd22d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YES</t>
   </si>
   <si>
     <t xml:space="preserve">asd dsdsd</t>
@@ -2683,11 +2695,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2866,11 +2878,11 @@
   </sheetPr>
   <dimension ref="A1:AAJ1001"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="ACV1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="ADH2" activeCellId="0" sqref="ADH2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="VF1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="VJ3" activeCellId="0" sqref="VJ3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.91015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16"/>
@@ -5033,16 +5045,16 @@
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>712</v>
@@ -5057,106 +5069,106 @@
         <v>8</v>
       </c>
       <c r="J2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="AL2" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="AM2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ2" s="0" t="s">
         <v>715</v>
       </c>
       <c r="AT2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BM2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BN2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BO2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BP2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BQ2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BR2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BS2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BT2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BU2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BW2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BY2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BZ2" s="0" t="s">
         <v>716</v>
@@ -5165,121 +5177,121 @@
         <v>716</v>
       </c>
       <c r="CB2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CC2" s="0" t="n">
         <v>123</v>
       </c>
       <c r="CE2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CF2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CG2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CH2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CI2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CK2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CL2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CM2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CN2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CO2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CP2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CQ2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CS2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CT2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CU2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CV2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CW2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CX2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CY2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CZ2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DA2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DB2" s="0" t="s">
         <v>717</v>
       </c>
       <c r="DD2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DE2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DF2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DG2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DH2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="EN2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="EO2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="EP2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="EQ2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="ES2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="EU2" s="0" t="s">
         <v>718</v>
       </c>
       <c r="EV2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="EW2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="EX2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="EY2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="EZ2" s="0" t="n">
         <v>12345</v>
@@ -5288,1036 +5300,1048 @@
         <v>719</v>
       </c>
       <c r="FB2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="FC2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="FD2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="FE2" s="0" t="s">
+        <v>720</v>
+      </c>
+      <c r="FF2" s="0" t="s">
+        <v>721</v>
       </c>
       <c r="FN2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="FO2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="FQ2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="FR2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="FS2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="FT2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="FU2" s="0" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="FV2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="FX2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="FY2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="FZ2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="GB2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="GC2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="GD2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="GF2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="GG2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="GI2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="GJ2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="GK2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="GL2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="GN2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="GP2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="GQ2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="GS2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="GT2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="GU2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="GX2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="GY2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="GZ2" s="0" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="HA2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HC2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HD2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HE2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HF2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HH2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HK2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HM2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="HP2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="HP2" s="2" t="n">
         <v>0.6875</v>
       </c>
-      <c r="HQ2" s="1" t="n">
+      <c r="HQ2" s="2" t="n">
         <v>0.333333333333333</v>
       </c>
-      <c r="HR2" s="1" t="n">
+      <c r="HR2" s="2" t="n">
         <v>0.6875</v>
       </c>
-      <c r="HS2" s="1" t="n">
+      <c r="HS2" s="2" t="n">
         <v>0.333333333333333</v>
       </c>
       <c r="HU2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HV2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="ID2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IE2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IG2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="II2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="IJ2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IK2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IL2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IM2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IN2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IO2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IP2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IQ2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IS2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IT2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IU2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IV2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IW2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IX2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="IY2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JA2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JB2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JC2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JD2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JE2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JF2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JG2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JH2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JI2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JM2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JN2" s="0" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="JO2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JQ2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JR2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JS2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JT2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JU2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JV2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JW2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JX2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JY2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="JZ2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KA2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KB2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KC2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KD2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KI2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KJ2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KL2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KM2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KN2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KO2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KP2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KQ2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KR2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KU2" s="0" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="KV2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="KX2" s="0" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="KY2" s="0" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="KZ2" s="0" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="LA2" s="0" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="LB2" s="0" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="LC2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="LD2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="LF2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="LH2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="LI2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="LJ2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="LK2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="LL2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="LM2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="LN2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="LO2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="LQ2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="LS2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="LT2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="LU2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="LV2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="LX2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="LZ2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="MA2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="MC2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="MG2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="MH2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="MI2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="MJ2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="MM2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="MN2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="MO2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="MP2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="MQ2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="MR2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="MS2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="NE2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="NH2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="NI2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="NI2" s="2" t="n">
         <v>0.6875</v>
       </c>
-      <c r="NJ2" s="1" t="n">
+      <c r="NJ2" s="2" t="n">
         <v>0.333333333333333</v>
       </c>
-      <c r="NK2" s="1" t="n">
+      <c r="NK2" s="2" t="n">
         <v>0.6875</v>
       </c>
-      <c r="NL2" s="1" t="n">
+      <c r="NL2" s="2" t="n">
         <v>0.333333333333333</v>
       </c>
       <c r="NM2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="NP2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="NQ2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="NR2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="NS2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="NT2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="NU2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="NV2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="NW2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="NX2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="NY2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="NZ2" s="0" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="OB2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="OC2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="OD2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="OE2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="OF2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="OG2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="OH2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="OI2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="OJ2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="OK2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="OL2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="OM2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="OO2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="OX2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="OY2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="OZ2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="PA2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="PB2" s="0" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="PE2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="PF2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="PG2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="PI2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="PJ2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="PK2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="PL2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="PO2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="PP2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="PQ2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="PT2" s="0" t="s">
+        <v>730</v>
       </c>
       <c r="QV2" s="0" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="QW2" s="0" t="s">
+        <v>732</v>
+      </c>
+      <c r="QX2" s="0" t="s">
+        <v>733</v>
+      </c>
+      <c r="QY2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="QZ2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="RA2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="RB2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="RC2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="RD2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="RE2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="RF2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="RG2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="RH2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="RI2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="RJ2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="RK2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="RL2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="RM2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="RN2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="RO2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="RP2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="RQ2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="RR2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="RT2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="RU2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="RV2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="RW2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="RX2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="RY2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="RZ2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="SC2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="SH2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="SI2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="SK2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="SL2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="SM2" s="0" t="s">
+        <v>734</v>
+      </c>
+      <c r="SN2" s="0" t="s">
+        <v>735</v>
+      </c>
+      <c r="SO2" s="0" t="s">
+        <v>736</v>
+      </c>
+      <c r="SP2" s="0" t="s">
+        <v>737</v>
+      </c>
+      <c r="SQ2" s="0" t="s">
+        <v>738</v>
+      </c>
+      <c r="SR2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="SS2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="SV2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="SW2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="SX2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="SZ2" s="0" t="s">
+        <v>739</v>
+      </c>
+      <c r="TC2" s="0" t="s">
+        <v>740</v>
+      </c>
+      <c r="TD2" s="0" t="s">
+        <v>741</v>
+      </c>
+      <c r="TE2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="TF2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="TG2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="TH2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="TI2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="TJ2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="TK2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="TL2" s="0" t="s">
+        <v>742</v>
+      </c>
+      <c r="TM2" s="0" t="s">
+        <v>743</v>
+      </c>
+      <c r="TN2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="TO2" s="0" t="s">
+        <v>744</v>
+      </c>
+      <c r="TQ2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="TR2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="TS2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="TT2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="TU2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="TV2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="TW2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="TZ2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="UA2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="UB2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="UC2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="UD2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="UG2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="UH2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="UI2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="UJ2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="UO2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="UQ2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="UR2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="US2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="UT2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="UZ2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="VA2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="VG2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="VJ2" s="0" t="s">
+        <v>745</v>
+      </c>
+      <c r="VM2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="VN2" s="0" t="s">
         <v>729</v>
       </c>
-      <c r="QX2" s="0" t="s">
-        <v>730</v>
-      </c>
-      <c r="QY2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="QZ2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="RA2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="RB2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="RC2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="RD2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="RE2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="RF2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="RG2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="RH2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="RI2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="RJ2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="RK2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="RL2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="RM2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="RN2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="RO2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="RP2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="RQ2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="RR2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="RT2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="RU2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="RV2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="RW2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="RX2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="RY2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="RZ2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="SC2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="SH2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="SI2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="SK2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="SL2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="SM2" s="0" t="s">
-        <v>731</v>
-      </c>
-      <c r="SN2" s="0" t="s">
-        <v>732</v>
-      </c>
-      <c r="SO2" s="0" t="s">
-        <v>733</v>
-      </c>
-      <c r="SP2" s="0" t="s">
-        <v>734</v>
-      </c>
-      <c r="SQ2" s="0" t="s">
-        <v>735</v>
-      </c>
-      <c r="SR2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="SS2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="SV2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="SW2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="SX2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="SZ2" s="0" t="s">
-        <v>736</v>
-      </c>
-      <c r="TC2" s="0" t="s">
-        <v>737</v>
-      </c>
-      <c r="TD2" s="0" t="s">
-        <v>738</v>
-      </c>
-      <c r="TE2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="TF2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="TG2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="TH2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="TI2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="TJ2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="TK2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="TL2" s="0" t="s">
-        <v>739</v>
-      </c>
-      <c r="TM2" s="0" t="s">
-        <v>740</v>
-      </c>
-      <c r="TN2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="TO2" s="0" t="s">
-        <v>741</v>
-      </c>
-      <c r="TQ2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="TR2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="TS2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="TT2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="TU2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="TV2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="TW2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="TZ2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="UA2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="UB2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="UC2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="UD2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="UG2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="UH2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="UI2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="UJ2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="UO2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="UQ2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="UR2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="US2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="UT2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="UZ2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="VA2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="VG2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="VM2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="VN2" s="0" t="s">
-        <v>727</v>
-      </c>
       <c r="VS2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="VT2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="VW2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="WA2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="WB2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="WC2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="WD2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="WE2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="WG2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="WH2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="WI2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="WJ2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="WK2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="WN2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="WO2" s="0" t="s">
-        <v>742</v>
+        <v>746</v>
       </c>
       <c r="WP2" s="0" t="s">
-        <v>743</v>
+        <v>747</v>
       </c>
       <c r="WR2" s="0" t="s">
-        <v>744</v>
+        <v>748</v>
       </c>
       <c r="WS2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="WT2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="WV2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="WX2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="XC2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="XD2" s="0" t="s">
-        <v>745</v>
+        <v>749</v>
       </c>
       <c r="XE2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="XF2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="XG2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="XH2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="XI2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="XJ2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="XK2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="XL2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="XL2" s="2" t="n">
         <v>0.6875</v>
       </c>
-      <c r="XM2" s="1" t="n">
+      <c r="XM2" s="2" t="n">
         <v>0.333333333333333</v>
       </c>
-      <c r="XN2" s="1" t="n">
+      <c r="XN2" s="2" t="n">
         <v>0.6875</v>
       </c>
-      <c r="XO2" s="1" t="n">
+      <c r="XO2" s="2" t="n">
         <v>0.333333333333333</v>
       </c>
       <c r="XQ2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="XS2" s="0" t="s">
-        <v>746</v>
+        <v>750</v>
       </c>
       <c r="XY2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="XZ2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="YC2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="YD2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="YE2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="YF2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="YG2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="YH2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="YI2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="YJ2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="YJ2" s="2" t="n">
         <v>0.6875</v>
       </c>
-      <c r="YK2" s="1" t="n">
+      <c r="YK2" s="2" t="n">
         <v>0.333333333333333</v>
       </c>
-      <c r="YL2" s="1" t="n">
+      <c r="YL2" s="2" t="n">
         <v>0.6875</v>
       </c>
-      <c r="YM2" s="1" t="n">
+      <c r="YM2" s="2" t="n">
         <v>0.333333333333333</v>
       </c>
       <c r="YR2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="YS2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="YT2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="YU2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="ZB2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="ZC2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="ZE2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="ZH2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="ZI2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="ZJ2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="ZS2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="ZU2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="ZV2" s="0" t="s">
-        <v>747</v>
-      </c>
-      <c r="ZW2" s="1" t="n">
+        <v>751</v>
+      </c>
+      <c r="ZW2" s="2" t="n">
         <v>0.6875</v>
       </c>
-      <c r="ZX2" s="1" t="n">
+      <c r="ZX2" s="2" t="n">
         <v>0.333333333333333</v>
       </c>
-      <c r="ZY2" s="1" t="n">
+      <c r="ZY2" s="2" t="n">
         <v>0.6875</v>
       </c>
-      <c r="ZZ2" s="1" t="n">
+      <c r="ZZ2" s="2" t="n">
         <v>0.333333333333333</v>
       </c>
       <c r="AAA2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AAB2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AAC2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AAD2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AAE2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="AAF2" s="2" t="n">
+      <c r="AAF2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AAG2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AAH2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AAI2" s="0" t="s">
-        <v>748</v>
+        <v>752</v>
       </c>
       <c r="AAJ2" s="0" t="n">
         <v>66000</v>
@@ -6408,6 +6432,7 @@
       <c r="ZZ18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F19" s="1"/>
       <c r="HP19" s="3"/>
       <c r="HQ19" s="3"/>
       <c r="NI19" s="3"/>
@@ -14941,7 +14966,7 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.51953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="44.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.76"/>
@@ -14949,10 +14974,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>749</v>
+        <v>753</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>750</v>
+        <v>754</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14960,7 +14985,7 @@
         <v>523</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>751</v>
+        <v>755</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14968,7 +14993,7 @@
         <v>176</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14976,7 +15001,7 @@
         <v>697</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>753</v>
+        <v>757</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14984,7 +15009,7 @@
         <v>531</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>754</v>
+        <v>758</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14992,7 +15017,7 @@
         <v>532</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>755</v>
+        <v>759</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15000,7 +15025,7 @@
         <v>160</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>756</v>
+        <v>760</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15008,7 +15033,7 @@
         <v>161</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>756</v>
+        <v>760</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15016,7 +15041,7 @@
         <v>642</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>757</v>
+        <v>761</v>
       </c>
     </row>
   </sheetData>
@@ -15041,7 +15066,7 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.51953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.12"/>
@@ -15049,10 +15074,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>749</v>
+        <v>753</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>750</v>
+        <v>754</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15060,7 +15085,7 @@
         <v>273</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>758</v>
+        <v>762</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15068,7 +15093,7 @@
         <v>156</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>759</v>
+        <v>763</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15076,7 +15101,7 @@
         <v>310</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>760</v>
+        <v>764</v>
       </c>
     </row>
   </sheetData>
@@ -15101,7 +15126,7 @@
       <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.51953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29"/>
@@ -15110,10 +15135,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>749</v>
+        <v>753</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>750</v>
+        <v>754</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15121,7 +15146,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>761</v>
+        <v>765</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15129,7 +15154,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>762</v>
+        <v>766</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15137,7 +15162,7 @@
         <v>105</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>763</v>
+        <v>767</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15153,7 +15178,7 @@
         <v>615</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>764</v>
+        <v>768</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15161,7 +15186,7 @@
         <v>711</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>765</v>
+        <v>769</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15169,15 +15194,15 @@
         <v>223</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>766</v>
+        <v>770</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>767</v>
+        <v>771</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>766</v>
+        <v>770</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15185,15 +15210,15 @@
         <v>372</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>766</v>
+        <v>770</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>768</v>
+        <v>772</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>766</v>
+        <v>770</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15201,15 +15226,15 @@
         <v>556</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>766</v>
+        <v>770</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>769</v>
+        <v>773</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>766</v>
+        <v>770</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15217,15 +15242,15 @@
         <v>622</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>766</v>
+        <v>770</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
+        <v>774</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>770</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15233,15 +15258,15 @@
         <v>635</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>766</v>
+        <v>770</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>771</v>
+        <v>775</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>766</v>
+        <v>770</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15249,15 +15274,15 @@
         <v>659</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>766</v>
+        <v>770</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>772</v>
+        <v>776</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>766</v>
+        <v>770</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15265,15 +15290,15 @@
         <v>698</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>766</v>
+        <v>770</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>773</v>
+        <v>777</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>766</v>
+        <v>770</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15284,10 +15309,10 @@
         <v>628</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>774</v>
+        <v>778</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>775</v>
+        <v>779</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15295,7 +15320,7 @@
         <v>629</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>776</v>
+        <v>780</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15303,7 +15328,7 @@
         <v>630</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>776</v>
+        <v>780</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15311,7 +15336,7 @@
         <v>631</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>776</v>
+        <v>780</v>
       </c>
     </row>
   </sheetData>
@@ -15336,7 +15361,7 @@
       <selection pane="topLeft" activeCell="A82" activeCellId="0" sqref="A82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.51953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="79.5"/>
@@ -15345,10 +15370,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>749</v>
+        <v>753</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>750</v>
+        <v>754</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15356,7 +15381,7 @@
         <v>519</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>777</v>
+        <v>781</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15364,7 +15389,7 @@
         <v>543</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>778</v>
+        <v>782</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15372,7 +15397,7 @@
         <v>441</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>778</v>
+        <v>782</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15380,7 +15405,7 @@
         <v>435</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>779</v>
+        <v>783</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15388,15 +15413,15 @@
         <v>581</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>780</v>
+        <v>784</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>781</v>
+        <v>785</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="17" t="s">
-        <v>782</v>
+        <v>786</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15404,7 +15429,7 @@
         <v>460</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>783</v>
+        <v>787</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15412,7 +15437,7 @@
         <v>540</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>784</v>
+        <v>788</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15420,7 +15445,7 @@
         <v>545</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>784</v>
+        <v>788</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15428,7 +15453,7 @@
         <v>547</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>784</v>
+        <v>788</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15436,7 +15461,7 @@
         <v>548</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>784</v>
+        <v>788</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15444,7 +15469,7 @@
         <v>586</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>785</v>
+        <v>789</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15452,7 +15477,7 @@
         <v>587</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>785</v>
+        <v>789</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15460,7 +15485,7 @@
         <v>589</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>785</v>
+        <v>789</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15468,7 +15493,7 @@
         <v>599</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>784</v>
+        <v>788</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15476,7 +15501,7 @@
         <v>653</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>786</v>
+        <v>790</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15484,7 +15509,7 @@
         <v>680</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>786</v>
+        <v>790</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15492,7 +15517,7 @@
         <v>683</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>786</v>
+        <v>790</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15500,7 +15525,7 @@
         <v>702</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>786</v>
+        <v>790</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15509,7 +15534,7 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="17" t="s">
-        <v>787</v>
+        <v>791</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15517,7 +15542,7 @@
         <v>15</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>788</v>
+        <v>792</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15525,7 +15550,7 @@
         <v>14</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>788</v>
+        <v>792</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15533,7 +15558,7 @@
         <v>147</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>789</v>
+        <v>793</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15541,7 +15566,7 @@
         <v>149</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>790</v>
+        <v>794</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15549,7 +15574,7 @@
         <v>276</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>791</v>
+        <v>795</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15557,7 +15582,7 @@
         <v>277</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>791</v>
+        <v>795</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15565,7 +15590,7 @@
         <v>278</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>791</v>
+        <v>795</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15573,7 +15598,7 @@
         <v>279</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>791</v>
+        <v>795</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15581,7 +15606,7 @@
         <v>305</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>792</v>
+        <v>796</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15589,7 +15614,7 @@
         <v>308</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>793</v>
+        <v>797</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15597,7 +15622,7 @@
         <v>314</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>794</v>
+        <v>798</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15605,7 +15630,7 @@
         <v>318</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>795</v>
+        <v>799</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15613,7 +15638,7 @@
         <v>319</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>794</v>
+        <v>798</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15621,7 +15646,7 @@
         <v>320</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>794</v>
+        <v>798</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15629,7 +15654,7 @@
         <v>321</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>794</v>
+        <v>798</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15637,7 +15662,7 @@
         <v>323</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>794</v>
+        <v>798</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15645,7 +15670,7 @@
         <v>324</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>794</v>
+        <v>798</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15653,7 +15678,7 @@
         <v>339</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>796</v>
+        <v>800</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15661,7 +15686,7 @@
         <v>369</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>797</v>
+        <v>801</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15669,7 +15694,7 @@
         <v>387</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>798</v>
+        <v>802</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15677,7 +15702,7 @@
         <v>388</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>798</v>
+        <v>802</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15685,7 +15710,7 @@
         <v>447</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>788</v>
+        <v>792</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15693,7 +15718,7 @@
         <v>448</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>788</v>
+        <v>792</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15701,7 +15726,7 @@
         <v>452</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>799</v>
+        <v>803</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15709,7 +15734,7 @@
         <v>455</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>788</v>
+        <v>792</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15717,7 +15742,7 @@
         <v>485</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>800</v>
+        <v>804</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15725,7 +15750,7 @@
         <v>487</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>800</v>
+        <v>804</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15733,7 +15758,7 @@
         <v>488</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>800</v>
+        <v>804</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15741,7 +15766,7 @@
         <v>491</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>800</v>
+        <v>804</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15749,7 +15774,7 @@
         <v>493</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>800</v>
+        <v>804</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15757,7 +15782,7 @@
         <v>524</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>800</v>
+        <v>804</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15765,7 +15790,7 @@
         <v>525</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>800</v>
+        <v>804</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15773,7 +15798,7 @@
         <v>526</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>800</v>
+        <v>804</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15781,7 +15806,7 @@
         <v>527</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>800</v>
+        <v>804</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15789,7 +15814,7 @@
         <v>529</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>800</v>
+        <v>804</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15797,7 +15822,7 @@
         <v>537</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>801</v>
+        <v>805</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15805,7 +15830,7 @@
         <v>538</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>801</v>
+        <v>805</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15813,7 +15838,7 @@
         <v>554</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>802</v>
+        <v>806</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15821,7 +15846,7 @@
         <v>580</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>788</v>
+        <v>792</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15829,7 +15854,7 @@
         <v>583</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>788</v>
+        <v>792</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15837,7 +15862,7 @@
         <v>588</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>802</v>
+        <v>806</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15845,7 +15870,7 @@
         <v>595</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>801</v>
+        <v>805</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15853,7 +15878,7 @@
         <v>596</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>801</v>
+        <v>805</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15861,7 +15886,7 @@
         <v>597</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>801</v>
+        <v>805</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15869,7 +15894,7 @@
         <v>598</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>801</v>
+        <v>805</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15877,7 +15902,7 @@
         <v>602</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>803</v>
+        <v>807</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15885,7 +15910,7 @@
         <v>607</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>801</v>
+        <v>805</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15893,7 +15918,7 @@
         <v>608</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>801</v>
+        <v>805</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15901,7 +15926,7 @@
         <v>609</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>788</v>
+        <v>792</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15909,7 +15934,7 @@
         <v>611</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>801</v>
+        <v>805</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15917,7 +15942,7 @@
         <v>614</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>801</v>
+        <v>805</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15925,7 +15950,7 @@
         <v>616</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>801</v>
+        <v>805</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15933,7 +15958,7 @@
         <v>617</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>801</v>
+        <v>805</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15941,7 +15966,7 @@
         <v>706</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>804</v>
+        <v>808</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15949,7 +15974,7 @@
         <v>707</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>805</v>
+        <v>809</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15957,7 +15982,7 @@
         <v>708</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>806</v>
+        <v>810</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15965,7 +15990,7 @@
         <v>709</v>
       </c>
       <c r="B80" s="11" t="s">
-        <v>807</v>
+        <v>811</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15973,7 +15998,7 @@
         <v>681</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>808</v>
+        <v>812</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15982,7 +16007,7 @@
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="17" t="s">
-        <v>809</v>
+        <v>813</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15990,7 +16015,7 @@
         <v>196</v>
       </c>
       <c r="B84" s="25" t="s">
-        <v>810</v>
+        <v>814</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15998,7 +16023,7 @@
         <v>365</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>811</v>
+        <v>815</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16006,7 +16031,7 @@
         <v>382</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>812</v>
+        <v>816</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16014,7 +16039,7 @@
         <v>383</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>812</v>
+        <v>816</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16022,7 +16047,7 @@
         <v>384</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>812</v>
+        <v>816</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16030,7 +16055,7 @@
         <v>385</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>812</v>
+        <v>816</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16038,7 +16063,7 @@
         <v>386</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>812</v>
+        <v>816</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16046,7 +16071,7 @@
         <v>442</v>
       </c>
       <c r="B91" s="26" t="s">
-        <v>810</v>
+        <v>814</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16054,7 +16079,7 @@
         <v>606</v>
       </c>
       <c r="B92" s="11" t="s">
-        <v>813</v>
+        <v>817</v>
       </c>
     </row>
   </sheetData>

</xml_diff>